<commit_message>
Fin del desarrollo de las pruebas
</commit_message>
<xml_diff>
--- a/src/test/resources/data/infoAlojamientos.xlsx
+++ b/src/test/resources/data/infoAlojamientos.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsnar\Downloads\juan\SQA\ScreenPlayReto\ScreenPlay-Abnb\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4624F187-2848-45AA-B388-576CA4099969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B92100-A642-4C72-ACA4-61E017BFF747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="1845" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Titulo</t>
   </si>
@@ -29,12 +29,22 @@
   </si>
   <si>
     <t>Precio</t>
+  </si>
+  <si>
+    <t>Nuevo Apto cerca al aeropuerto con parqueadero.</t>
+  </si>
+  <si>
+    <t>Angee Julieth</t>
+  </si>
+  <si>
+    <t>$996,889 COP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,23 +410,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>